<commit_message>
removed utf-8 chars from setup.cfg implemented ModuleParser.py w/ test test_module_parser.py
</commit_message>
<xml_diff>
--- a/tests/data/ci_v2_data.xlsx
+++ b/tests/data/ci_v2_data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10308"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10413"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/csxds/workspaces/python/ngmodel/tests/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/csxds/workspaces/python/eam-core/tests/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05758EC0-EFAA-4F4A-8087-354A62E730B5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8697A28B-10E2-FA42-8B02-1CA4B364C37D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="7520" yWindow="2980" windowWidth="28800" windowHeight="17540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="params" sheetId="7" r:id="rId1"/>
@@ -32,15 +32,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="40">
   <si>
     <t>variable</t>
   </si>
   <si>
     <t>scenario</t>
-  </si>
-  <si>
-    <t>S1</t>
   </si>
   <si>
     <t>type</t>
@@ -553,7 +550,7 @@
   <dimension ref="A1:S9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B23" sqref="B23"/>
+      <selection activeCell="S10" sqref="S10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -566,70 +563,70 @@
         <v>1</v>
       </c>
       <c r="C1" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="E1" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="E1" s="9" t="s">
+      <c r="F1" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="G1" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="G1" s="4" t="s">
+      <c r="H1" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="H1" s="4" t="s">
+      <c r="I1" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="I1" s="4" t="s">
+      <c r="J1" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="J1" s="9" t="s">
+      <c r="K1" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="K1" s="4" t="s">
+      <c r="L1" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="L1" s="4" t="s">
+      <c r="M1" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="M1" s="4" t="s">
+      <c r="N1" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="N1" s="4" t="s">
+      <c r="O1" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="O1" s="4" t="s">
-        <v>15</v>
-      </c>
       <c r="P1" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q1" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="Q1" s="7" t="s">
-        <v>35</v>
-      </c>
       <c r="R1" s="8" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="S1" s="10" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="2" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B2" s="2"/>
       <c r="C2" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D2" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="D2" s="2" t="s">
-        <v>17</v>
-      </c>
       <c r="E2" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F2" s="2">
         <v>0</v>
@@ -644,7 +641,7 @@
         <v>43617</v>
       </c>
       <c r="J2" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="K2" s="2"/>
       <c r="L2" s="2"/>
@@ -652,28 +649,31 @@
       <c r="N2" s="2"/>
       <c r="O2" s="2"/>
       <c r="P2" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="Q2" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="R2" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="Q2" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="R2" s="6" t="s">
-        <v>39</v>
+      <c r="S2">
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B3" s="2"/>
       <c r="C3" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D3" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="D3" s="2" t="s">
-        <v>17</v>
-      </c>
       <c r="E3" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F3" s="2">
         <v>0</v>
@@ -688,7 +688,7 @@
         <v>43617</v>
       </c>
       <c r="J3" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="K3" s="2"/>
       <c r="L3" s="2"/>
@@ -696,16 +696,19 @@
       <c r="N3" s="2"/>
       <c r="O3" s="2"/>
       <c r="Q3" s="6" t="s">
-        <v>36</v>
+        <v>35</v>
+      </c>
+      <c r="S3">
+        <v>2</v>
       </c>
     </row>
     <row r="4" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B4" s="2"/>
       <c r="C4" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D4" s="2"/>
       <c r="E4" s="2">
@@ -724,21 +727,24 @@
         <v>42522</v>
       </c>
       <c r="J4" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="K4" s="2"/>
       <c r="L4" s="2"/>
       <c r="M4" s="2"/>
       <c r="N4" s="2"/>
       <c r="O4" s="2"/>
+      <c r="S4">
+        <v>3</v>
+      </c>
     </row>
     <row r="5" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B5" s="2"/>
       <c r="C5" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E5" s="5">
         <f>5*8*1000000</f>
@@ -757,21 +763,24 @@
         <v>43617</v>
       </c>
       <c r="J5" s="5" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="K5" s="2"/>
       <c r="L5" s="2"/>
       <c r="M5" s="2"/>
       <c r="N5" s="2"/>
       <c r="O5" s="2"/>
+      <c r="S5">
+        <v>4</v>
+      </c>
     </row>
     <row r="6" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B6" s="2"/>
       <c r="C6" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E6" s="2">
         <v>0.5</v>
@@ -789,42 +798,27 @@
         <v>43617</v>
       </c>
       <c r="J6" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="K6" s="2"/>
       <c r="L6" s="2"/>
       <c r="M6" s="2"/>
       <c r="N6" s="2"/>
       <c r="O6" s="2"/>
+      <c r="S6">
+        <v>5</v>
+      </c>
     </row>
     <row r="7" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A7" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="E7" s="2">
-        <v>0.5</v>
-      </c>
-      <c r="F7" s="2">
-        <v>-0.2</v>
-      </c>
-      <c r="G7" s="2">
-        <v>0.1</v>
-      </c>
-      <c r="H7" s="2">
-        <v>0.05</v>
-      </c>
-      <c r="I7" s="3">
-        <v>43617</v>
-      </c>
-      <c r="J7" s="2" t="s">
-        <v>32</v>
-      </c>
+      <c r="A7" s="2"/>
+      <c r="B7" s="2"/>
+      <c r="C7" s="2"/>
+      <c r="E7" s="2"/>
+      <c r="F7" s="2"/>
+      <c r="G7" s="2"/>
+      <c r="H7" s="2"/>
+      <c r="I7" s="3"/>
+      <c r="J7" s="2"/>
       <c r="K7" s="2"/>
       <c r="L7" s="2"/>
       <c r="M7" s="2"/>
@@ -852,10 +846,10 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>19</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>20</v>
       </c>
     </row>
   </sheetData>
@@ -876,7 +870,7 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B1" s="1">
         <v>2</v>

</xml_diff>

<commit_message>
- [x] updates on ModuleParser.py: find data files in directory, filter UI params from table.csv - [x] update test
- [x] ADDED openpyxl to dependencies
</commit_message>
<xml_diff>
--- a/tests/data/ci_v2_data.xlsx
+++ b/tests/data/ci_v2_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/csxds/workspaces/python/eam-core/tests/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8697A28B-10E2-FA42-8B02-1CA4B364C37D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B83A629-6B7C-9D46-A264-E0640ABCE9F0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7520" yWindow="2980" windowWidth="28800" windowHeight="17540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="params" sheetId="7" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="40">
   <si>
     <t>variable</t>
   </si>
@@ -550,7 +550,7 @@
   <dimension ref="A1:S9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="S10" sqref="S10"/>
+      <selection activeCell="Q5" sqref="Q5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -805,6 +805,9 @@
       <c r="M6" s="2"/>
       <c r="N6" s="2"/>
       <c r="O6" s="2"/>
+      <c r="Q6" t="s">
+        <v>35</v>
+      </c>
       <c r="S6">
         <v>5</v>
       </c>

</xml_diff>

<commit_message>
added tests for process ids
</commit_message>
<xml_diff>
--- a/tests/data/ci_v2_data.xlsx
+++ b/tests/data/ci_v2_data.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView activeTab="0" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible" windowHeight="8964" windowWidth="17280" xWindow="732" yWindow="732"/>
+    <workbookView activeTab="0" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible" windowHeight="12576" windowWidth="23256" xWindow="-108" yWindow="-108"/>
   </bookViews>
   <sheets>
     <sheet name="params" sheetId="1" state="visible" r:id="rId1"/>
@@ -11,7 +11,7 @@
     <sheet name="metadata" sheetId="3" state="visible" r:id="rId3"/>
   </sheets>
   <definedNames/>
-  <calcPr calcId="191029" fullCalcOnLoad="1"/>
+  <calcPr calcId="0" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
@@ -81,16 +81,12 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="7">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf borderId="0" fillId="0" fontId="0" numFmtId="14" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf borderId="0" fillId="2" fontId="2" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf borderId="0" fillId="0" fontId="3" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf borderId="0" fillId="2" fontId="2" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf borderId="0" fillId="3" fontId="2" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf borderId="0" fillId="3" fontId="2" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf borderId="0" fillId="4" fontId="2" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
@@ -405,103 +401,103 @@
   <dimension ref="A1:S9"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
-      <selection activeCell="T3" sqref="T3"/>
+      <selection activeCell="S2" sqref="S2:S7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultColWidth="11.5546875" defaultRowHeight="14.4"/>
   <sheetData>
     <row r="1">
-      <c r="A1" s="7" t="inlineStr">
+      <c r="A1" s="4" t="inlineStr">
         <is>
           <t>variable</t>
         </is>
       </c>
-      <c r="B1" s="7" t="inlineStr">
+      <c r="B1" s="4" t="inlineStr">
         <is>
           <t>scenario</t>
         </is>
       </c>
-      <c r="C1" s="7" t="inlineStr">
+      <c r="C1" s="4" t="inlineStr">
         <is>
           <t>type</t>
         </is>
       </c>
-      <c r="D1" s="7" t="inlineStr">
+      <c r="D1" s="4" t="inlineStr">
         <is>
           <t>param</t>
         </is>
       </c>
-      <c r="E1" s="9" t="inlineStr">
+      <c r="E1" s="5" t="inlineStr">
         <is>
           <t>ref value</t>
         </is>
       </c>
-      <c r="F1" s="7" t="inlineStr">
+      <c r="F1" s="4" t="inlineStr">
         <is>
           <t>mean growth</t>
         </is>
       </c>
-      <c r="G1" s="7" t="inlineStr">
+      <c r="G1" s="4" t="inlineStr">
         <is>
           <t>initial_value_proportional_variation</t>
         </is>
       </c>
-      <c r="H1" s="7" t="inlineStr">
+      <c r="H1" s="4" t="inlineStr">
         <is>
           <t>variability growth</t>
         </is>
       </c>
-      <c r="I1" s="7" t="inlineStr">
+      <c r="I1" s="4" t="inlineStr">
         <is>
           <t>ref date</t>
         </is>
       </c>
-      <c r="J1" s="9" t="inlineStr">
+      <c r="J1" s="5" t="inlineStr">
         <is>
           <t>unit</t>
         </is>
       </c>
-      <c r="K1" s="7" t="inlineStr">
+      <c r="K1" s="4" t="inlineStr">
         <is>
           <t>label</t>
         </is>
       </c>
-      <c r="L1" s="7" t="inlineStr">
+      <c r="L1" s="4" t="inlineStr">
         <is>
           <t>source</t>
         </is>
       </c>
-      <c r="M1" s="7" t="inlineStr">
+      <c r="M1" s="4" t="inlineStr">
         <is>
           <t>comment</t>
         </is>
       </c>
-      <c r="N1" s="7" t="inlineStr">
+      <c r="N1" s="4" t="inlineStr">
         <is>
           <t>control</t>
         </is>
       </c>
-      <c r="O1" s="7" t="inlineStr">
+      <c r="O1" s="4" t="inlineStr">
         <is>
           <t>scenario notes</t>
         </is>
       </c>
-      <c r="P1" s="9" t="inlineStr">
+      <c r="P1" s="5" t="inlineStr">
         <is>
           <t>description</t>
         </is>
       </c>
-      <c r="Q1" s="7" t="inlineStr">
+      <c r="Q1" s="4" t="inlineStr">
         <is>
           <t>ui variable</t>
         </is>
       </c>
-      <c r="R1" s="9" t="inlineStr">
+      <c r="R1" s="5" t="inlineStr">
         <is>
           <t>user name</t>
         </is>
       </c>
-      <c r="S1" s="10" t="inlineStr">
+      <c r="S1" s="6" t="inlineStr">
         <is>
           <t>id</t>
         </is>
@@ -537,7 +533,7 @@
       <c r="H2" t="n">
         <v>0.05</v>
       </c>
-      <c r="I2" s="3" t="n">
+      <c r="I2" s="2" t="n">
         <v>43617</v>
       </c>
       <c r="J2" t="inlineStr">
@@ -545,23 +541,23 @@
           <t>W</t>
         </is>
       </c>
-      <c r="P2" s="6" t="inlineStr">
+      <c r="P2" s="3" t="inlineStr">
         <is>
           <t>what does it mean? How do collect this info?</t>
         </is>
       </c>
-      <c r="Q2" s="6" t="inlineStr">
+      <c r="Q2" s="3" t="inlineStr">
         <is>
           <t>x</t>
         </is>
       </c>
-      <c r="R2" s="6" t="inlineStr">
+      <c r="R2" s="3" t="inlineStr">
         <is>
           <t>power draw of laptop</t>
         </is>
       </c>
       <c r="S2" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3">
@@ -594,7 +590,7 @@
       <c r="H3" t="n">
         <v>0.05</v>
       </c>
-      <c r="I3" s="3" t="n">
+      <c r="I3" s="2" t="n">
         <v>43617</v>
       </c>
       <c r="J3" t="inlineStr">
@@ -602,13 +598,13 @@
           <t>minute</t>
         </is>
       </c>
-      <c r="Q3" s="6" t="inlineStr">
+      <c r="Q3" s="3" t="inlineStr">
         <is>
           <t>x</t>
         </is>
       </c>
       <c r="S3" t="n">
-        <v>8</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4">
@@ -634,7 +630,7 @@
       <c r="H4" t="n">
         <v>0.1</v>
       </c>
-      <c r="I4" s="3" t="n">
+      <c r="I4" s="2" t="n">
         <v>42522</v>
       </c>
       <c r="J4" t="inlineStr">
@@ -643,7 +639,7 @@
         </is>
       </c>
       <c r="S4" t="n">
-        <v>9</v>
+        <v>2</v>
       </c>
     </row>
     <row r="5">
@@ -657,7 +653,7 @@
           <t>exp</t>
         </is>
       </c>
-      <c r="E5" s="6" t="n">
+      <c r="E5" s="3" t="n">
         <v>40000000</v>
       </c>
       <c r="F5" t="n">
@@ -669,16 +665,16 @@
       <c r="H5" t="n">
         <v>0.05</v>
       </c>
-      <c r="I5" s="3" t="n">
+      <c r="I5" s="2" t="n">
         <v>43617</v>
       </c>
-      <c r="J5" s="6" t="inlineStr">
+      <c r="J5" s="3" t="inlineStr">
         <is>
           <t>bps</t>
         </is>
       </c>
       <c r="S5" t="n">
-        <v>10</v>
+        <v>3</v>
       </c>
     </row>
     <row r="6">
@@ -704,7 +700,7 @@
       <c r="H6" t="n">
         <v>0.05</v>
       </c>
-      <c r="I6" s="3" t="n">
+      <c r="I6" s="2" t="n">
         <v>43617</v>
       </c>
       <c r="J6" t="inlineStr">
@@ -713,7 +709,7 @@
         </is>
       </c>
       <c r="S6" t="n">
-        <v>11</v>
+        <v>4</v>
       </c>
     </row>
     <row r="7">
@@ -744,7 +740,7 @@
       <c r="H7" t="n">
         <v>0.05</v>
       </c>
-      <c r="I7" s="3" t="n">
+      <c r="I7" s="2" t="n">
         <v>43617</v>
       </c>
       <c r="J7" t="inlineStr">
@@ -753,12 +749,12 @@
         </is>
       </c>
       <c r="S7" t="n">
-        <v>12</v>
+        <v>5</v>
       </c>
     </row>
     <row r="8"/>
     <row r="9">
-      <c r="E9" s="6" t="n"/>
+      <c r="E9" s="3" t="n"/>
     </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
@@ -779,7 +775,7 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" customHeight="1" defaultColWidth="14.44140625" defaultRowHeight="15"/>
   <sheetData>
-    <row customHeight="1" ht="15" r="1" s="2">
+    <row customHeight="1" ht="15" r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
           <t>31.7.18</t>
@@ -810,7 +806,7 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" customHeight="1" defaultColWidth="14.44140625" defaultRowHeight="15"/>
   <sheetData>
-    <row customHeight="1" ht="15" r="1" s="2">
+    <row customHeight="1" ht="15" r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
           <t>version</t>

</xml_diff>

<commit_message>
added logging to antlr parser fail on syntax errors remove side effect on log levelname in colored formatter add flag: formula_checks to yaml_runner.py update tests
https://github.com/sust-cs-uob/dimpact-model-streaming/issues/4
</commit_message>
<xml_diff>
--- a/tests/data/ci_v2_data.xlsx
+++ b/tests/data/ci_v2_data.xlsx
@@ -401,7 +401,7 @@
   <dimension ref="A1:S9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q4" sqref="Q4"/>
+      <selection activeCell="R7" sqref="R7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15"/>
@@ -711,6 +711,11 @@
       <c r="Q6" s="3" t="inlineStr">
         <is>
           <t>p</t>
+        </is>
+      </c>
+      <c r="R6" s="3" t="inlineStr">
+        <is>
+          <t>carbon intensity</t>
         </is>
       </c>
       <c r="S6" t="n">

</xml_diff>

<commit_message>
country renamed to group, countries renamed to groupings
</commit_message>
<xml_diff>
--- a/tests/data/ci_v2_data.xlsx
+++ b/tests/data/ci_v2_data.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView activeTab="0" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible" windowHeight="14780" windowWidth="27560" xWindow="0" yWindow="460"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="0" yWindow="460" windowWidth="27560" windowHeight="14780" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet name="params" sheetId="1" state="visible" r:id="rId1"/>
@@ -79,21 +79,89 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="7">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="14" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf borderId="0" fillId="2" fontId="2" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf borderId="0" fillId="3" fontId="2" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf borderId="0" fillId="4" fontId="2" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle builtinId="0" name="Normal" xfId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium2"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -790,7 +858,7 @@
       <c r="E9" s="3" t="n"/>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
@@ -806,9 +874,9 @@
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" customHeight="1" defaultColWidth="14.5" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15" customHeight="1"/>
   <sheetData>
-    <row customHeight="1" ht="15" r="1">
+    <row r="1" ht="15" customHeight="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
           <t>31.7.18</t>
@@ -821,7 +889,7 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
@@ -837,9 +905,9 @@
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" customHeight="1" defaultColWidth="14.5" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15" customHeight="1"/>
   <sheetData>
-    <row customHeight="1" ht="15" r="1">
+    <row r="1" ht="15" customHeight="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
           <t>version</t>
@@ -850,6 +918,6 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
implemented multiple correlation, sensitivity analysis should work
</commit_message>
<xml_diff>
--- a/tests/data/ci_v2_data.xlsx
+++ b/tests/data/ci_v2_data.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="0" yWindow="460" windowWidth="27560" windowHeight="14780" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView activeTab="0" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible" windowHeight="14780" windowWidth="27560" xWindow="0" yWindow="460"/>
   </bookViews>
   <sheets>
     <sheet name="params" sheetId="1" state="visible" r:id="rId1"/>
@@ -79,89 +79,21 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
   <cellXfs count="7">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="14" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf borderId="0" fillId="2" fontId="2" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf borderId="0" fillId="3" fontId="2" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf borderId="0" fillId="4" fontId="2" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle builtinId="0" name="Normal" xfId="0"/>
   </cellStyles>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
-  <colors>
-    <indexedColors>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008000"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00808000"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="00C0C0C0"/>
-      <rgbColor rgb="00808080"/>
-      <rgbColor rgb="009999FF"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00FFFFCC"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00660066"/>
-      <rgbColor rgb="00FF8080"/>
-      <rgbColor rgb="000066CC"/>
-      <rgbColor rgb="00CCCCFF"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="0000CCFF"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00CCFFCC"/>
-      <rgbColor rgb="00FFFF99"/>
-      <rgbColor rgb="0099CCFF"/>
-      <rgbColor rgb="00FF99CC"/>
-      <rgbColor rgb="00CC99FF"/>
-      <rgbColor rgb="00FFCC99"/>
-      <rgbColor rgb="003366FF"/>
-      <rgbColor rgb="0033CCCC"/>
-      <rgbColor rgb="0099CC00"/>
-      <rgbColor rgb="00FFCC00"/>
-      <rgbColor rgb="00FF9900"/>
-      <rgbColor rgb="00FF6600"/>
-      <rgbColor rgb="00666699"/>
-      <rgbColor rgb="00969696"/>
-      <rgbColor rgb="00003366"/>
-      <rgbColor rgb="00339966"/>
-      <rgbColor rgb="00003300"/>
-      <rgbColor rgb="00333300"/>
-      <rgbColor rgb="00993300"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00333399"/>
-      <rgbColor rgb="00333333"/>
-    </indexedColors>
-  </colors>
+  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium2"/>
 </styleSheet>
 </file>
 
@@ -858,7 +790,7 @@
       <c r="E9" s="3" t="n"/>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
@@ -874,9 +806,9 @@
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr baseColWidth="10" customHeight="1" defaultColWidth="14.5" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" ht="15" customHeight="1">
+    <row customHeight="1" ht="15" r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
           <t>31.7.18</t>
@@ -889,7 +821,7 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
@@ -905,9 +837,9 @@
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr baseColWidth="10" customHeight="1" defaultColWidth="14.5" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" ht="15" customHeight="1">
+    <row customHeight="1" ht="15" r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
           <t>version</t>
@@ -918,6 +850,6 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
</xml_diff>